<commit_message>
Changes done by Khubim
</commit_message>
<xml_diff>
--- a/Working_Diary.xlsx
+++ b/Working_Diary.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7F0DD0-B3DD-47DC-8B99-040B428930A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE7E27A-356A-4A8A-A6CA-EC2137532E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10848" yWindow="2472" windowWidth="12252" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Team Member</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>28/2/2022</t>
+  </si>
+  <si>
+    <t>Load the dataset and checked for Null values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renamed the columns and  Cleaned city and country </t>
   </si>
 </sst>
 </file>
@@ -49,7 +55,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -90,7 +96,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,17 +438,17 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -453,23 +459,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
       <c r="C3" s="1">
         <v>44564</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -477,7 +489,7 @@
         <v>44595</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -485,7 +497,7 @@
         <v>44623</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -496,7 +508,7 @@
         <v>44624</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
diary updated by murthy
</commit_message>
<xml_diff>
--- a/Working_Diary.xlsx
+++ b/Working_Diary.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE7E27A-356A-4A8A-A6CA-EC2137532E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10848" yWindow="2472" windowWidth="12252" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10850" yWindow="2470" windowWidth="12250" windowHeight="8880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>Team Member</t>
   </si>
@@ -48,12 +47,15 @@
   </si>
   <si>
     <t xml:space="preserve">Renamed the columns and  Cleaned city and country </t>
+  </si>
+  <si>
+    <t>Worked on Tableau</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -190,23 +192,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -242,23 +227,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -434,21 +402,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -459,7 +427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -470,7 +438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -481,7 +449,7 @@
         <v>44564</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -489,7 +457,7 @@
         <v>44595</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -497,7 +465,7 @@
         <v>44623</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -508,7 +476,7 @@
         <v>44624</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -517,6 +485,61 @@
       </c>
       <c r="C7" s="3">
         <v>44625</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44626</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44628</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44629</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44630</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dashboard and working diary Pushed
</commit_message>
<xml_diff>
--- a/Working_Diary.xlsx
+++ b/Working_Diary.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5F5C06-0742-4C87-AAE9-AA8883CB9592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948DF69F-F37E-4669-B8C8-8EAF0C6AAE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>Team Member</t>
   </si>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t>Dashboard finalisation - Final touch up to make things clearer and better</t>
+  </si>
+  <si>
+    <t>Khubim Chhetri</t>
+  </si>
+  <si>
+    <t>Dashboard working ,visualisation layout design</t>
+  </si>
+  <si>
+    <t>Interactions and design done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final Dashboard committed </t>
   </si>
 </sst>
 </file>
@@ -70,7 +82,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -110,7 +122,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -450,20 +462,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,7 +486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -485,7 +497,7 @@
         <v>44620</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -496,7 +508,7 @@
         <v>44621</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -507,7 +519,7 @@
         <v>44622</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -518,7 +530,7 @@
         <v>44623</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -529,7 +541,7 @@
         <v>44624</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -540,7 +552,7 @@
         <v>44625</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -551,7 +563,7 @@
         <v>44626</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -562,7 +574,7 @@
         <v>44628</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -573,7 +585,7 @@
         <v>44629</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -584,7 +596,7 @@
         <v>44630</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -595,7 +607,7 @@
         <v>44631</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -606,7 +618,7 @@
         <v>44633</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -617,7 +629,7 @@
         <v>44634</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -626,6 +638,39 @@
       </c>
       <c r="C15" s="3">
         <v>44636</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="3">
+        <v>44638</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="3">
+        <v>44639</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="3">
+        <v>44640</v>
       </c>
     </row>
   </sheetData>

</xml_diff>